<commit_message>
Refined Reports to be faster
</commit_message>
<xml_diff>
--- a/src/lib/server/reports/templates/TEMPLATE_A1-InTheProgram.xlsx
+++ b/src/lib/server/reports/templates/TEMPLATE_A1-InTheProgram.xlsx
@@ -645,10 +645,10 @@
       <xdr:rowOff>66600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>64080</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>905760</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -661,8 +661,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9523800" y="266760"/>
-          <a:ext cx="1350360" cy="787320"/>
+          <a:off x="12040920" y="266760"/>
+          <a:ext cx="1349640" cy="786600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -683,10 +683,10 @@
       <xdr:rowOff>95400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>277920</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1167480</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>34920</xdr:rowOff>
+      <xdr:rowOff>34200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -699,8 +699,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3589560" y="95400"/>
-          <a:ext cx="1139760" cy="1139760"/>
+          <a:off x="4091040" y="95400"/>
+          <a:ext cx="1139040" cy="1139040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -896,16 +896,23 @@
   </sheetPr>
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="17.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="22.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="24.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>